<commit_message>
Chinh sua Activity Bar Chart
</commit_message>
<xml_diff>
--- a/Bao cao/Activities Bar Char.xlsx
+++ b/Bao cao/Activities Bar Char.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="64">
   <si>
     <t>Công việc</t>
   </si>
@@ -115,6 +115,9 @@
     <t>Quản lý chương trình khuyến mãi (DFD mức 1, DFD tổng quát)</t>
   </si>
   <si>
+    <t>Quản lý nhà cung cấp (DFD mức 1, DFD tổng quát)</t>
+  </si>
+  <si>
     <t>Thiết kế giao diện (Quản lý sản phẩm, danh sách hóa đơn, quản lý phiếu nhập, quản lý chương trình khuyến mãi, quản lý khách hàng, đăng nhập, quản lý tài khoản, popup thêm tài khoản)</t>
   </si>
   <si>
@@ -163,6 +166,9 @@
     <t>Sequence Diagram (Quản lý chương trình khuyến mãi)</t>
   </si>
   <si>
+    <t>Sequence Diagram (Quản lý nhà cung cấp)</t>
+  </si>
+  <si>
     <t>Activity Diagram</t>
   </si>
   <si>
@@ -172,7 +178,31 @@
     <t>ERD</t>
   </si>
   <si>
-    <t>Usecase</t>
+    <t>Usecase (Vẽ Diagram, Đặc tả các chức năng của Báo cáo thống kê)</t>
+  </si>
+  <si>
+    <t>Usecase (Đặc tả các chức năng của Quản lý nhân viên)</t>
+  </si>
+  <si>
+    <t>Usecase (Đặc tả các chức năng của Quản lý tài khoản)</t>
+  </si>
+  <si>
+    <t>Usecase (Đặc tả các chức năng của Quản lý sản phẩm)</t>
+  </si>
+  <si>
+    <t>Usecase (Đặc tả các chức năng của Quản lý kho)</t>
+  </si>
+  <si>
+    <t>Usecase (Đặc tả các chức năng của Quản lý khách hàng)</t>
+  </si>
+  <si>
+    <t>Usecase (Đặc tả các chức năng của Quản lý hóa đơn)</t>
+  </si>
+  <si>
+    <t>Usecase (Đặc tả các chức năng của Quản lý chương trình khuyến mãi)</t>
+  </si>
+  <si>
+    <t>Usecase (Đặc tả các chức năng của Quản lý nhà cung cấp)</t>
   </si>
   <si>
     <t>Chạy thử phầm mềm</t>
@@ -183,9 +213,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="176" formatCode="dd/mm"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="dd/mm"/>
+    <numFmt numFmtId="177" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
@@ -229,9 +259,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -245,6 +282,22 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -252,16 +305,46 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -283,9 +366,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -299,21 +388,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -321,50 +395,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -381,187 +411,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -575,17 +605,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -605,20 +640,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -664,11 +696,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -677,159 +707,159 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -841,25 +871,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="58" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1197,10 +1221,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:CB43"/>
+  <dimension ref="A1:CB53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="AL44" sqref="AL44:AR44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90740740740741" defaultRowHeight="14.4"/>
@@ -1214,8 +1238,8 @@
   <sheetData>
     <row r="1" spans="2:2">
       <c r="B1">
-        <f>COUNTIF(B3:B43,"Kỷ")</f>
-        <v>4</v>
+        <f>COUNTIF(B3:B54,"Kỷ")</f>
+        <v>5</v>
       </c>
     </row>
     <row r="2" ht="15" spans="1:80">
@@ -1372,35 +1396,35 @@
       <c r="AY2" s="2">
         <v>44169</v>
       </c>
-      <c r="AZ2" s="12"/>
-      <c r="BA2" s="12"/>
-      <c r="BB2" s="12"/>
-      <c r="BC2" s="12"/>
-      <c r="BD2" s="12"/>
-      <c r="BE2" s="12"/>
-      <c r="BF2" s="12"/>
-      <c r="BG2" s="12"/>
-      <c r="BH2" s="12"/>
-      <c r="BI2" s="12"/>
-      <c r="BJ2" s="12"/>
-      <c r="BK2" s="12"/>
-      <c r="BL2" s="12"/>
-      <c r="BM2" s="12"/>
-      <c r="BN2" s="12"/>
-      <c r="BO2" s="12"/>
-      <c r="BP2" s="12"/>
-      <c r="BQ2" s="12"/>
-      <c r="BR2" s="12"/>
-      <c r="BS2" s="12"/>
-      <c r="BT2" s="12"/>
-      <c r="BU2" s="12"/>
-      <c r="BV2" s="12"/>
-      <c r="BW2" s="12"/>
-      <c r="BX2" s="12"/>
-      <c r="BY2" s="12"/>
-      <c r="BZ2" s="12"/>
-      <c r="CA2" s="12"/>
-      <c r="CB2" s="12"/>
+      <c r="AZ2" s="10"/>
+      <c r="BA2" s="10"/>
+      <c r="BB2" s="10"/>
+      <c r="BC2" s="10"/>
+      <c r="BD2" s="10"/>
+      <c r="BE2" s="10"/>
+      <c r="BF2" s="10"/>
+      <c r="BG2" s="10"/>
+      <c r="BH2" s="10"/>
+      <c r="BI2" s="10"/>
+      <c r="BJ2" s="10"/>
+      <c r="BK2" s="10"/>
+      <c r="BL2" s="10"/>
+      <c r="BM2" s="10"/>
+      <c r="BN2" s="10"/>
+      <c r="BO2" s="10"/>
+      <c r="BP2" s="10"/>
+      <c r="BQ2" s="10"/>
+      <c r="BR2" s="10"/>
+      <c r="BS2" s="10"/>
+      <c r="BT2" s="10"/>
+      <c r="BU2" s="10"/>
+      <c r="BV2" s="10"/>
+      <c r="BW2" s="10"/>
+      <c r="BX2" s="10"/>
+      <c r="BY2" s="10"/>
+      <c r="BZ2" s="10"/>
+      <c r="CA2" s="10"/>
+      <c r="CB2" s="10"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
@@ -1420,7 +1444,7 @@
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="4">
@@ -1434,7 +1458,7 @@
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="4">
@@ -1448,7 +1472,7 @@
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="4">
@@ -1462,7 +1486,7 @@
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="4">
@@ -1476,7 +1500,7 @@
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="4">
@@ -1490,7 +1514,7 @@
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="4">
@@ -1504,7 +1528,7 @@
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="4">
@@ -1518,7 +1542,7 @@
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="4">
@@ -1571,11 +1595,11 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>7</v>
+      <c r="B15" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="C15" s="4">
         <v>44137</v>
@@ -1585,10 +1609,10 @@
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="4">
@@ -1599,10 +1623,10 @@
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C17" s="4">
@@ -1613,10 +1637,10 @@
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="4">
@@ -1627,10 +1651,10 @@
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="4">
@@ -1641,10 +1665,10 @@
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="4">
@@ -1655,10 +1679,10 @@
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C21" s="4">
@@ -1669,10 +1693,10 @@
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="4">
@@ -1683,58 +1707,58 @@
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="4">
+        <v>44137</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="C23" s="4">
-        <v>44143</v>
-      </c>
-      <c r="D23" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" t="s">
-        <v>19</v>
       </c>
       <c r="C24" s="4">
         <v>44143</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="3" t="s">
+      <c r="A25" t="s">
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C25" s="4">
         <v>44143</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25">
         <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" t="s">
+      <c r="A26" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C26" s="4">
         <v>44143</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="5">
         <v>6</v>
       </c>
     </row>
@@ -1743,40 +1767,40 @@
         <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C27" s="4">
         <v>44143</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27">
         <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="3" t="s">
+      <c r="A28" t="s">
         <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C28" s="4">
         <v>44143</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" t="s">
+      <c r="A29" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C29" s="4">
         <v>44143</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29">
         <v>6</v>
       </c>
     </row>
@@ -1785,40 +1809,40 @@
         <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C30" s="4">
         <v>44143</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="3" t="s">
+      <c r="A31" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="9">
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="4">
+        <v>44143</v>
+      </c>
+      <c r="D31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="4">
         <v>44152</v>
       </c>
-      <c r="D31" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="9">
-        <v>44152</v>
-      </c>
-      <c r="D32">
+      <c r="D32" s="5">
         <v>7</v>
       </c>
     </row>
@@ -1826,13 +1850,13 @@
       <c r="A33" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" s="9">
+      <c r="B33" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="4">
         <v>44152</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33">
         <v>7</v>
       </c>
     </row>
@@ -1840,13 +1864,13 @@
       <c r="A34" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="9">
+      <c r="B34" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="4">
         <v>44152</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="5">
         <v>7</v>
       </c>
     </row>
@@ -1854,13 +1878,13 @@
       <c r="A35" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="9">
+      <c r="B35" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="4">
         <v>44152</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35">
         <v>7</v>
       </c>
     </row>
@@ -1868,13 +1892,13 @@
       <c r="A36" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36" s="9">
+      <c r="B36" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="4">
         <v>44152</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="5">
         <v>7</v>
       </c>
     </row>
@@ -1882,13 +1906,13 @@
       <c r="A37" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" s="9">
+      <c r="B37" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="4">
         <v>44152</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37">
         <v>7</v>
       </c>
     </row>
@@ -1896,41 +1920,41 @@
       <c r="A38" t="s">
         <v>48</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="4">
+        <v>44152</v>
+      </c>
+      <c r="D38" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C38" s="9">
+      <c r="C39" s="4">
         <v>44152</v>
       </c>
-      <c r="D38">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="9">
-        <v>44155</v>
-      </c>
-      <c r="D39" s="6">
+      <c r="D39">
         <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="3" t="s">
+      <c r="A40" t="s">
         <v>50</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C40" s="9">
-        <v>44155</v>
-      </c>
-      <c r="D40" s="6">
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="4">
+        <v>44152</v>
+      </c>
+      <c r="D40">
         <v>7</v>
       </c>
     </row>
@@ -1938,233 +1962,403 @@
       <c r="A41" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="4">
+        <v>44155</v>
+      </c>
+      <c r="D41" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="4">
+        <v>44155</v>
+      </c>
+      <c r="D42" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C41" s="9">
+      <c r="C43" s="4">
         <v>44152</v>
       </c>
-      <c r="D41" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" t="s">
-        <v>52</v>
-      </c>
-      <c r="B42" s="6" t="s">
+      <c r="D43" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>54</v>
+      </c>
+      <c r="B44" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C42" s="9">
+      <c r="C44" s="4">
         <v>44156</v>
       </c>
-      <c r="D42" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" ht="16.8" spans="1:4">
-      <c r="A43" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="D44" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>55</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="4">
+        <v>44156</v>
+      </c>
+      <c r="D45" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>56</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" s="4">
+        <v>44156</v>
+      </c>
+      <c r="D46" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>57</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="4">
+        <v>44156</v>
+      </c>
+      <c r="D47" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="4">
+        <v>44156</v>
+      </c>
+      <c r="D48" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>59</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" s="4">
+        <v>44156</v>
+      </c>
+      <c r="D49" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>60</v>
+      </c>
+      <c r="B50" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="11">
+      <c r="C50" s="4">
+        <v>44156</v>
+      </c>
+      <c r="D50" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>61</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" s="4">
+        <v>44156</v>
+      </c>
+      <c r="D51" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>62</v>
+      </c>
+      <c r="B52" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" s="4">
+        <v>44156</v>
+      </c>
+      <c r="D52" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" ht="16.8" spans="1:4">
+      <c r="A53" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B53" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53" s="9">
         <v>44164</v>
       </c>
-      <c r="D43">
+      <c r="D53">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="Y24:AD24">
-    <cfRule type="expression" priority="48">
-      <formula>IF(AND(Y$2&gt;=$C24,Y$2&lt;=$C24+$D24-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="47">
-      <formula>IF(AND(Y$2&gt;=$C24,Y$2&lt;=$C24+$D24-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="46">
-      <formula>IF(AND(Y$2&gt;=$C24,Y$2&lt;=$C24+$D24-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="45">
-      <formula>IF(AND(Y$2&gt;=$C24,Y$2&lt;=$C24+$D24-1),TRUE,FALSE)</formula>
+  <conditionalFormatting sqref="S23:W23">
+    <cfRule type="expression" priority="8">
+      <formula>IF(AND(S$2&gt;=$C23,S$2&lt;=$C23+$D23-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="7">
+      <formula>IF(AND(S$2&gt;=$C23,S$2&lt;=$C23+$D23-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="6">
+      <formula>IF(AND(S$2&gt;=$C23,S$2&lt;=$C23+$D23-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="5">
+      <formula>IF(AND(S$2&gt;=$C23,S$2&lt;=$C23+$D23-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y25:AD25">
-    <cfRule type="expression" priority="44">
+    <cfRule type="expression" dxfId="1" priority="53">
       <formula>IF(AND(Y$2&gt;=$C25,Y$2&lt;=$C25+$D25-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="43">
+    <cfRule type="expression" dxfId="1" priority="54">
       <formula>IF(AND(Y$2&gt;=$C25,Y$2&lt;=$C25+$D25-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="42">
+    <cfRule type="expression" dxfId="0" priority="55">
       <formula>IF(AND(Y$2&gt;=$C25,Y$2&lt;=$C25+$D25-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="41">
+    <cfRule type="expression" priority="56">
       <formula>IF(AND(Y$2&gt;=$C25,Y$2&lt;=$C25+$D25-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y26:AD26">
-    <cfRule type="expression" priority="40">
+    <cfRule type="expression" dxfId="1" priority="49">
       <formula>IF(AND(Y$2&gt;=$C26,Y$2&lt;=$C26+$D26-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="39">
+    <cfRule type="expression" dxfId="1" priority="50">
       <formula>IF(AND(Y$2&gt;=$C26,Y$2&lt;=$C26+$D26-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="38">
+    <cfRule type="expression" dxfId="0" priority="51">
       <formula>IF(AND(Y$2&gt;=$C26,Y$2&lt;=$C26+$D26-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="37">
+    <cfRule type="expression" priority="52">
       <formula>IF(AND(Y$2&gt;=$C26,Y$2&lt;=$C26+$D26-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y27:AD27">
-    <cfRule type="expression" priority="36">
+    <cfRule type="expression" dxfId="1" priority="45">
       <formula>IF(AND(Y$2&gt;=$C27,Y$2&lt;=$C27+$D27-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="35">
+    <cfRule type="expression" dxfId="1" priority="46">
       <formula>IF(AND(Y$2&gt;=$C27,Y$2&lt;=$C27+$D27-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="34">
+    <cfRule type="expression" dxfId="0" priority="47">
       <formula>IF(AND(Y$2&gt;=$C27,Y$2&lt;=$C27+$D27-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="33">
+    <cfRule type="expression" priority="48">
       <formula>IF(AND(Y$2&gt;=$C27,Y$2&lt;=$C27+$D27-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y28:AD28">
-    <cfRule type="expression" priority="32">
+    <cfRule type="expression" dxfId="1" priority="41">
       <formula>IF(AND(Y$2&gt;=$C28,Y$2&lt;=$C28+$D28-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="31">
+    <cfRule type="expression" dxfId="1" priority="42">
       <formula>IF(AND(Y$2&gt;=$C28,Y$2&lt;=$C28+$D28-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="30">
+    <cfRule type="expression" dxfId="0" priority="43">
       <formula>IF(AND(Y$2&gt;=$C28,Y$2&lt;=$C28+$D28-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="29">
+    <cfRule type="expression" priority="44">
       <formula>IF(AND(Y$2&gt;=$C28,Y$2&lt;=$C28+$D28-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y29:AD29">
-    <cfRule type="expression" priority="28">
+    <cfRule type="expression" dxfId="1" priority="37">
       <formula>IF(AND(Y$2&gt;=$C29,Y$2&lt;=$C29+$D29-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="27">
+    <cfRule type="expression" dxfId="1" priority="38">
       <formula>IF(AND(Y$2&gt;=$C29,Y$2&lt;=$C29+$D29-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="26">
+    <cfRule type="expression" dxfId="0" priority="39">
       <formula>IF(AND(Y$2&gt;=$C29,Y$2&lt;=$C29+$D29-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="25">
+    <cfRule type="expression" priority="40">
       <formula>IF(AND(Y$2&gt;=$C29,Y$2&lt;=$C29+$D29-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y30:AD30">
-    <cfRule type="expression" priority="24">
+    <cfRule type="expression" dxfId="1" priority="33">
       <formula>IF(AND(Y$2&gt;=$C30,Y$2&lt;=$C30+$D30-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="23">
+    <cfRule type="expression" dxfId="1" priority="34">
       <formula>IF(AND(Y$2&gt;=$C30,Y$2&lt;=$C30+$D30-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="22">
+    <cfRule type="expression" dxfId="0" priority="35">
       <formula>IF(AND(Y$2&gt;=$C30,Y$2&lt;=$C30+$D30-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="21">
+    <cfRule type="expression" priority="36">
       <formula>IF(AND(Y$2&gt;=$C30,Y$2&lt;=$C30+$D30-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH32:AN32">
-    <cfRule type="expression" priority="20">
-      <formula>IF(AND(AH$2&gt;=$C32,AH$2&lt;=$C32+$D32-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="19">
-      <formula>IF(AND(AH$2&gt;=$C32,AH$2&lt;=$C32+$D32-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="18">
-      <formula>IF(AND(AH$2&gt;=$C32,AH$2&lt;=$C32+$D32-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="17">
-      <formula>IF(AND(AH$2&gt;=$C32,AH$2&lt;=$C32+$D32-1),TRUE,FALSE)</formula>
+  <conditionalFormatting sqref="Y31:AD31">
+    <cfRule type="expression" dxfId="1" priority="29">
+      <formula>IF(AND(Y$2&gt;=$C31,Y$2&lt;=$C31+$D31-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="30">
+      <formula>IF(AND(Y$2&gt;=$C31,Y$2&lt;=$C31+$D31-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="31">
+      <formula>IF(AND(Y$2&gt;=$C31,Y$2&lt;=$C31+$D31-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" priority="32">
+      <formula>IF(AND(Y$2&gt;=$C31,Y$2&lt;=$C31+$D31-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH33:AN33">
-    <cfRule type="expression" priority="16">
+    <cfRule type="expression" dxfId="1" priority="25">
       <formula>IF(AND(AH$2&gt;=$C33,AH$2&lt;=$C33+$D33-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="15">
+    <cfRule type="expression" dxfId="1" priority="26">
       <formula>IF(AND(AH$2&gt;=$C33,AH$2&lt;=$C33+$D33-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="14">
+    <cfRule type="expression" dxfId="0" priority="27">
       <formula>IF(AND(AH$2&gt;=$C33,AH$2&lt;=$C33+$D33-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="13">
+    <cfRule type="expression" priority="28">
       <formula>IF(AND(AH$2&gt;=$C33,AH$2&lt;=$C33+$D33-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH34:AN34">
-    <cfRule type="expression" priority="12">
+    <cfRule type="expression" dxfId="1" priority="21">
       <formula>IF(AND(AH$2&gt;=$C34,AH$2&lt;=$C34+$D34-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="11">
+    <cfRule type="expression" dxfId="1" priority="22">
       <formula>IF(AND(AH$2&gt;=$C34,AH$2&lt;=$C34+$D34-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="10">
+    <cfRule type="expression" dxfId="0" priority="23">
       <formula>IF(AND(AH$2&gt;=$C34,AH$2&lt;=$C34+$D34-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="9">
+    <cfRule type="expression" priority="24">
       <formula>IF(AND(AH$2&gt;=$C34,AH$2&lt;=$C34+$D34-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH35:AN35">
-    <cfRule type="expression" priority="8">
+    <cfRule type="expression" dxfId="1" priority="17">
       <formula>IF(AND(AH$2&gt;=$C35,AH$2&lt;=$C35+$D35-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="7">
+    <cfRule type="expression" dxfId="1" priority="18">
       <formula>IF(AND(AH$2&gt;=$C35,AH$2&lt;=$C35+$D35-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="6">
+    <cfRule type="expression" dxfId="0" priority="19">
       <formula>IF(AND(AH$2&gt;=$C35,AH$2&lt;=$C35+$D35-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="5">
+    <cfRule type="expression" priority="20">
       <formula>IF(AND(AH$2&gt;=$C35,AH$2&lt;=$C35+$D35-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH36:AN36">
-    <cfRule type="expression" priority="4">
+    <cfRule type="expression" dxfId="1" priority="13">
       <formula>IF(AND(AH$2&gt;=$C36,AH$2&lt;=$C36+$D36-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="1" priority="14">
       <formula>IF(AND(AH$2&gt;=$C36,AH$2&lt;=$C36+$D36-1),TRUE,FALSE)</formula>
     </cfRule>
+    <cfRule type="expression" dxfId="0" priority="15">
+      <formula>IF(AND(AH$2&gt;=$C36,AH$2&lt;=$C36+$D36-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" priority="16">
+      <formula>IF(AND(AH$2&gt;=$C36,AH$2&lt;=$C36+$D36-1),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH37:AN37">
+    <cfRule type="expression" dxfId="1" priority="9">
+      <formula>IF(AND(AH$2&gt;=$C37,AH$2&lt;=$C37+$D37-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="10">
+      <formula>IF(AND(AH$2&gt;=$C37,AH$2&lt;=$C37+$D37-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="11">
+      <formula>IF(AND(AH$2&gt;=$C37,AH$2&lt;=$C37+$D37-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" priority="12">
+      <formula>IF(AND(AH$2&gt;=$C37,AH$2&lt;=$C37+$D37-1),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH40:AN40">
+    <cfRule type="expression" dxfId="1" priority="4">
+      <formula>IF(AND(AH$2&gt;=$C40,AH$2&lt;=$C40+$D40-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>IF(AND(AH$2&gt;=$C40,AH$2&lt;=$C40+$D40-1),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL44:AR44">
     <cfRule type="expression" dxfId="1" priority="2">
-      <formula>IF(AND(AH$2&gt;=$C36,AH$2&lt;=$C36+$D36-1),TRUE,FALSE)</formula>
+      <formula>IF(AND(AL$2&gt;=$C44,AL$2&lt;=$C44+$D44-1),TRUE,FALSE)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="1">
-      <formula>IF(AND(AH$2&gt;=$C36,AH$2&lt;=$C36+$D36-1),TRUE,FALSE)</formula>
+      <formula>IF(AND(AL$2&gt;=$C44,AL$2&lt;=$C44+$D44-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:AU15">
-    <cfRule type="expression" dxfId="0" priority="54">
+    <cfRule type="expression" dxfId="0" priority="62">
       <formula>IF(AND(E$2&gt;=$C3,E$2&lt;=$C3+$D3-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:AU23 E31:AU31 E39:AU39">
-    <cfRule type="expression" dxfId="0" priority="51">
+  <conditionalFormatting sqref="E3:AU22 E32:AU32 E24:AU24 E41:AU41">
+    <cfRule type="expression" dxfId="0" priority="59">
       <formula>IF(AND(E$2&gt;=$C3,E$2&lt;=$C3+$D3-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" priority="52">
+    <cfRule type="expression" priority="60">
       <formula>IF(AND(E$2&gt;=$C3,E$2&lt;=$C3+$D3-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:AU23 E31:AU31 E37:AU114">
-    <cfRule type="expression" dxfId="1" priority="50">
+  <conditionalFormatting sqref="E3:AU22 E45:AU51 E53:AU54 E32:AU32 E56:AU113 E38:AU39 E41:AU43 E24:AU24">
+    <cfRule type="expression" dxfId="1" priority="58">
       <formula>IF(AND(E$2&gt;=$C3,E$2&lt;=$C3+$D3-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:AY23 E31:AY31 E37:AY95">
-    <cfRule type="expression" dxfId="1" priority="49">
+  <conditionalFormatting sqref="E3:AY22 E45:AY51 E53:AY54 E32:AY32 E56:AY94 E38:AY39 E41:AY43 E24:AY24">
+    <cfRule type="expression" dxfId="1" priority="57">
       <formula>IF(AND(E$2&gt;=$C3,E$2&lt;=$C3+$D3-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Xoa bang luong trong database
</commit_message>
<xml_diff>
--- a/Bao cao/Activities Bar Char.xlsx
+++ b/Bao cao/Activities Bar Char.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="73">
   <si>
     <t>Công việc</t>
   </si>
@@ -91,31 +91,58 @@
     <t>DFD mức 0 (Quản lý khách hàng, Quản lý hóa đơn, Quản lý chương trình khuyến mãi)</t>
   </si>
   <si>
-    <t>Báo cáo thống kê (DFD mức 1, DFD tổng quát)</t>
-  </si>
-  <si>
-    <t>Quản lý nhân viên (DFD mức 1, DFD tổng quát)</t>
-  </si>
-  <si>
-    <t>Quản lý tài khoản (DFD mức 1, DFD tổng quát)</t>
-  </si>
-  <si>
-    <t>Quản lý sản phẩm (DFD mức 1, DFD tổng quát)</t>
-  </si>
-  <si>
-    <t>Quản lý kho (DFD mức 1, DFD tổng quát)</t>
-  </si>
-  <si>
-    <t>Quản lý khách hàng (DFD mức 1, DFD tổng quát)</t>
-  </si>
-  <si>
-    <t>Quản lý hóa đơn (DFD mức 1, DFD tổng quát)</t>
-  </si>
-  <si>
-    <t>Quản lý chương trình khuyến mãi (DFD mức 1, DFD tổng quát)</t>
-  </si>
-  <si>
-    <t>Quản lý nhà cung cấp (DFD mức 1, DFD tổng quát)</t>
+    <t>Tiếp nhận hồ sơ nhân viên</t>
+  </si>
+  <si>
+    <t>Quản lý phiếu nhập</t>
+  </si>
+  <si>
+    <t>Thống kê doanh thu</t>
+  </si>
+  <si>
+    <t>Lập hóa đơn</t>
+  </si>
+  <si>
+    <t>Tổ chức khuyến mãi</t>
+  </si>
+  <si>
+    <t>Kiểm kê sản phẩm lỗi</t>
+  </si>
+  <si>
+    <t>Kiểm kê hàng tồn kho</t>
+  </si>
+  <si>
+    <t>Quản lý ca làm nhân viên</t>
+  </si>
+  <si>
+    <t>Quản lý tủ đồ</t>
+  </si>
+  <si>
+    <t>Lập phiếu xuất</t>
+  </si>
+  <si>
+    <t>Phân loại hàng theo danh mục</t>
+  </si>
+  <si>
+    <t>Cấp tài khoản nhân viên</t>
+  </si>
+  <si>
+    <t>Tiếp nhận khách hàng</t>
+  </si>
+  <si>
+    <t>Quản lý sản phẩm</t>
+  </si>
+  <si>
+    <t>Giữ trả xe</t>
+  </si>
+  <si>
+    <t>Quản lý nhà cung cấp</t>
+  </si>
+  <si>
+    <t>Thống kê lợi nhuận</t>
+  </si>
+  <si>
+    <t>Quản lý chức vụ</t>
   </si>
   <si>
     <t>Thiết kế giao diện (Quản lý sản phẩm, danh sách hóa đơn, quản lý phiếu nhập, quản lý chương trình khuyến mãi, quản lý khách hàng, đăng nhập, quản lý tài khoản, popup thêm tài khoản)</t>
@@ -213,12 +240,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="dd/mm"/>
+    <numFmt numFmtId="176" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="177" formatCode="dd/mm"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="m/d/yyyy;@"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -259,16 +286,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -283,6 +310,30 @@
     <font>
       <b/>
       <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -306,7 +357,59 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -319,82 +422,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -411,187 +438,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -602,71 +629,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -688,8 +650,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -702,20 +679,70 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -725,130 +752,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -859,7 +886,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -883,7 +910,7 @@
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -942,14 +969,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FF00B050"/>
+          <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1221,10 +1248,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:CB53"/>
+  <dimension ref="A1:CB63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="AL44" sqref="AL44:AR44"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90740740740741" defaultRowHeight="14.4"/>
@@ -1239,7 +1266,7 @@
     <row r="1" spans="2:2">
       <c r="B1">
         <f>COUNTIF(B3:B54,"Kỷ")</f>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" ht="15" spans="1:80">
@@ -1598,9 +1625,7 @@
       <c r="A15" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>23</v>
-      </c>
+      <c r="B15" s="7"/>
       <c r="C15" s="4">
         <v>44137</v>
       </c>
@@ -1612,9 +1637,7 @@
       <c r="A16" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="B16" s="7"/>
       <c r="C16" s="4">
         <v>44137</v>
       </c>
@@ -1626,9 +1649,7 @@
       <c r="A17" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="B17" s="7"/>
       <c r="C17" s="4">
         <v>44137</v>
       </c>
@@ -1640,9 +1661,7 @@
       <c r="A18" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>11</v>
-      </c>
+      <c r="B18" s="7"/>
       <c r="C18" s="4">
         <v>44137</v>
       </c>
@@ -1654,9 +1673,7 @@
       <c r="A19" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="B19" s="7"/>
       <c r="C19" s="4">
         <v>44137</v>
       </c>
@@ -1668,9 +1685,7 @@
       <c r="A20" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>15</v>
-      </c>
+      <c r="B20" s="7"/>
       <c r="C20" s="4">
         <v>44137</v>
       </c>
@@ -1682,9 +1697,7 @@
       <c r="A21" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="B21" s="7"/>
       <c r="C21" s="4">
         <v>44137</v>
       </c>
@@ -1696,9 +1709,7 @@
       <c r="A22" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="B22" s="7"/>
       <c r="C22" s="4">
         <v>44137</v>
       </c>
@@ -1710,9 +1721,7 @@
       <c r="A23" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
+      <c r="B23"/>
       <c r="C23" s="4">
         <v>44137</v>
       </c>
@@ -1720,295 +1729,200 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="4">
-        <v>44143</v>
-      </c>
-      <c r="D24" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+    </row>
+    <row r="25" spans="1:1">
       <c r="A25" t="s">
         <v>35</v>
       </c>
-      <c r="B25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="4">
-        <v>44143</v>
-      </c>
-      <c r="D25">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="3" t="s">
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
         <v>36</v>
       </c>
-      <c r="B26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="4">
-        <v>44143</v>
-      </c>
-      <c r="D26" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+    </row>
+    <row r="27" spans="1:1">
       <c r="A27" t="s">
         <v>37</v>
       </c>
-      <c r="B27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="4">
-        <v>44143</v>
-      </c>
-      <c r="D27">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+    </row>
+    <row r="28" spans="1:1">
       <c r="A28" t="s">
         <v>38</v>
       </c>
-      <c r="B28" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="4">
-        <v>44143</v>
-      </c>
-      <c r="D28" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="3" t="s">
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
         <v>39</v>
       </c>
-      <c r="B29" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="4">
-        <v>44143</v>
-      </c>
-      <c r="D29">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+    </row>
+    <row r="30" spans="1:1">
       <c r="A30" t="s">
         <v>40</v>
       </c>
-      <c r="B30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="4">
-        <v>44143</v>
-      </c>
-      <c r="D30" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+    </row>
+    <row r="31" spans="1:1">
       <c r="A31" t="s">
         <v>41</v>
       </c>
-      <c r="B31" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" s="4">
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="4">
         <v>44143</v>
       </c>
-      <c r="D31">
+      <c r="D34" s="5">
         <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" s="4">
-        <v>44152</v>
-      </c>
-      <c r="D32" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" s="4">
-        <v>44152</v>
-      </c>
-      <c r="D33">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" s="4">
-        <v>44152</v>
-      </c>
-      <c r="D34" s="5">
-        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="4">
+        <v>44143</v>
+      </c>
+      <c r="D35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" s="4">
-        <v>44152</v>
-      </c>
-      <c r="D35">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" t="s">
-        <v>46</v>
-      </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="4">
-        <v>44152</v>
+        <v>44143</v>
       </c>
       <c r="D36" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>47</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>15</v>
+        <v>46</v>
+      </c>
+      <c r="B37" t="s">
+        <v>13</v>
       </c>
       <c r="C37" s="4">
-        <v>44152</v>
+        <v>44143</v>
       </c>
       <c r="D37">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" s="4">
+        <v>44143</v>
+      </c>
+      <c r="D38" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B38" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C38" s="4">
-        <v>44152</v>
-      </c>
-      <c r="D38" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" t="s">
-        <v>49</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>19</v>
+      <c r="B39" t="s">
+        <v>9</v>
       </c>
       <c r="C39" s="4">
-        <v>44152</v>
+        <v>44143</v>
       </c>
       <c r="D39">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="4">
+        <v>44143</v>
+      </c>
+      <c r="D40" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
         <v>50</v>
       </c>
-      <c r="B40" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" s="4">
-        <v>44152</v>
-      </c>
-      <c r="D40">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>5</v>
+      <c r="B41" t="s">
+        <v>17</v>
       </c>
       <c r="C41" s="4">
-        <v>44155</v>
-      </c>
-      <c r="D41" s="5">
-        <v>7</v>
+        <v>44143</v>
+      </c>
+      <c r="D41">
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="4">
+        <v>44152</v>
+      </c>
+      <c r="D42" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
         <v>52</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C42" s="4">
-        <v>44155</v>
-      </c>
-      <c r="D42" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>23</v>
+      <c r="B43" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="C43" s="4">
         <v>44152</v>
       </c>
-      <c r="D43" s="5">
+      <c r="D43">
         <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C44" s="4">
-        <v>44156</v>
+        <v>44152</v>
       </c>
       <c r="D44" s="5">
         <v>7</v>
@@ -2016,27 +1930,27 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C45" s="4">
-        <v>44156</v>
-      </c>
-      <c r="D45" s="5">
+        <v>44152</v>
+      </c>
+      <c r="D45">
         <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C46" s="4">
-        <v>44156</v>
+        <v>44152</v>
       </c>
       <c r="D46" s="5">
         <v>7</v>
@@ -2044,27 +1958,27 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C47" s="4">
-        <v>44156</v>
-      </c>
-      <c r="D47" s="5">
+        <v>44152</v>
+      </c>
+      <c r="D47">
         <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C48" s="4">
-        <v>44156</v>
+        <v>44152</v>
       </c>
       <c r="D48" s="5">
         <v>7</v>
@@ -2072,293 +1986,433 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C49" s="4">
-        <v>44156</v>
-      </c>
-      <c r="D49" s="5">
+        <v>44152</v>
+      </c>
+      <c r="D49">
         <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" s="4">
+        <v>44152</v>
+      </c>
+      <c r="D50">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B51" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="4">
+        <v>44155</v>
+      </c>
+      <c r="D51" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" s="4">
+        <v>44155</v>
+      </c>
+      <c r="D52" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53" s="4">
+        <v>44152</v>
+      </c>
+      <c r="D53" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C54" s="4">
+        <v>44156</v>
+      </c>
+      <c r="D54" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
+        <v>64</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" s="4">
+        <v>44156</v>
+      </c>
+      <c r="D55" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>65</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C56" s="4">
+        <v>44156</v>
+      </c>
+      <c r="D56" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" s="4">
+        <v>44156</v>
+      </c>
+      <c r="D57" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" t="s">
+        <v>67</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="4">
+        <v>44156</v>
+      </c>
+      <c r="D58" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
+        <v>68</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C59" s="4">
+        <v>44156</v>
+      </c>
+      <c r="D59" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>69</v>
+      </c>
+      <c r="B60" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C50" s="4">
+      <c r="C60" s="4">
         <v>44156</v>
       </c>
-      <c r="D50" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" t="s">
-        <v>61</v>
-      </c>
-      <c r="B51" s="7" t="s">
+      <c r="D60" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>70</v>
+      </c>
+      <c r="B61" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C51" s="4">
+      <c r="C61" s="4">
         <v>44156</v>
       </c>
-      <c r="D51" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" t="s">
-        <v>62</v>
-      </c>
-      <c r="B52" t="s">
-        <v>7</v>
-      </c>
-      <c r="C52" s="4">
+      <c r="D61" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>71</v>
+      </c>
+      <c r="B62" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" s="4">
         <v>44156</v>
       </c>
-      <c r="D52" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="53" ht="16.8" spans="1:4">
-      <c r="A53" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B53" t="s">
+      <c r="D62" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" ht="16.8" spans="1:4">
+      <c r="A63" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B63" t="s">
         <v>13</v>
       </c>
-      <c r="C53" s="9">
+      <c r="C63" s="9">
         <v>44164</v>
       </c>
-      <c r="D53">
+      <c r="D63">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="S23:W23">
+    <cfRule type="expression" dxfId="0" priority="5">
+      <formula>IF(AND(S$2&gt;=$C23,S$2&lt;=$C23+$D23-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="6">
+      <formula>IF(AND(S$2&gt;=$C23,S$2&lt;=$C23+$D23-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="7">
+      <formula>IF(AND(S$2&gt;=$C23,S$2&lt;=$C23+$D23-1),TRUE,FALSE)</formula>
+    </cfRule>
     <cfRule type="expression" priority="8">
       <formula>IF(AND(S$2&gt;=$C23,S$2&lt;=$C23+$D23-1),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="7">
-      <formula>IF(AND(S$2&gt;=$C23,S$2&lt;=$C23+$D23-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="6">
-      <formula>IF(AND(S$2&gt;=$C23,S$2&lt;=$C23+$D23-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="5">
-      <formula>IF(AND(S$2&gt;=$C23,S$2&lt;=$C23+$D23-1),TRUE,FALSE)</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y25:AD25">
-    <cfRule type="expression" dxfId="1" priority="53">
-      <formula>IF(AND(Y$2&gt;=$C25,Y$2&lt;=$C25+$D25-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="54">
-      <formula>IF(AND(Y$2&gt;=$C25,Y$2&lt;=$C25+$D25-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="55">
-      <formula>IF(AND(Y$2&gt;=$C25,Y$2&lt;=$C25+$D25-1),TRUE,FALSE)</formula>
+  <conditionalFormatting sqref="Y35:AD35">
+    <cfRule type="expression" dxfId="0" priority="53">
+      <formula>IF(AND(Y$2&gt;=$C35,Y$2&lt;=$C35+$D35-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="54">
+      <formula>IF(AND(Y$2&gt;=$C35,Y$2&lt;=$C35+$D35-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="55">
+      <formula>IF(AND(Y$2&gt;=$C35,Y$2&lt;=$C35+$D35-1),TRUE,FALSE)</formula>
     </cfRule>
     <cfRule type="expression" priority="56">
-      <formula>IF(AND(Y$2&gt;=$C25,Y$2&lt;=$C25+$D25-1),TRUE,FALSE)</formula>
+      <formula>IF(AND(Y$2&gt;=$C35,Y$2&lt;=$C35+$D35-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y26:AD26">
-    <cfRule type="expression" dxfId="1" priority="49">
-      <formula>IF(AND(Y$2&gt;=$C26,Y$2&lt;=$C26+$D26-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="50">
-      <formula>IF(AND(Y$2&gt;=$C26,Y$2&lt;=$C26+$D26-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="51">
-      <formula>IF(AND(Y$2&gt;=$C26,Y$2&lt;=$C26+$D26-1),TRUE,FALSE)</formula>
+  <conditionalFormatting sqref="Y36:AD36">
+    <cfRule type="expression" dxfId="0" priority="49">
+      <formula>IF(AND(Y$2&gt;=$C36,Y$2&lt;=$C36+$D36-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="50">
+      <formula>IF(AND(Y$2&gt;=$C36,Y$2&lt;=$C36+$D36-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="51">
+      <formula>IF(AND(Y$2&gt;=$C36,Y$2&lt;=$C36+$D36-1),TRUE,FALSE)</formula>
     </cfRule>
     <cfRule type="expression" priority="52">
-      <formula>IF(AND(Y$2&gt;=$C26,Y$2&lt;=$C26+$D26-1),TRUE,FALSE)</formula>
+      <formula>IF(AND(Y$2&gt;=$C36,Y$2&lt;=$C36+$D36-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y27:AD27">
-    <cfRule type="expression" dxfId="1" priority="45">
-      <formula>IF(AND(Y$2&gt;=$C27,Y$2&lt;=$C27+$D27-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="46">
-      <formula>IF(AND(Y$2&gt;=$C27,Y$2&lt;=$C27+$D27-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="47">
-      <formula>IF(AND(Y$2&gt;=$C27,Y$2&lt;=$C27+$D27-1),TRUE,FALSE)</formula>
+  <conditionalFormatting sqref="Y37:AD37">
+    <cfRule type="expression" dxfId="0" priority="45">
+      <formula>IF(AND(Y$2&gt;=$C37,Y$2&lt;=$C37+$D37-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="46">
+      <formula>IF(AND(Y$2&gt;=$C37,Y$2&lt;=$C37+$D37-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="47">
+      <formula>IF(AND(Y$2&gt;=$C37,Y$2&lt;=$C37+$D37-1),TRUE,FALSE)</formula>
     </cfRule>
     <cfRule type="expression" priority="48">
-      <formula>IF(AND(Y$2&gt;=$C27,Y$2&lt;=$C27+$D27-1),TRUE,FALSE)</formula>
+      <formula>IF(AND(Y$2&gt;=$C37,Y$2&lt;=$C37+$D37-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y28:AD28">
-    <cfRule type="expression" dxfId="1" priority="41">
-      <formula>IF(AND(Y$2&gt;=$C28,Y$2&lt;=$C28+$D28-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="42">
-      <formula>IF(AND(Y$2&gt;=$C28,Y$2&lt;=$C28+$D28-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="43">
-      <formula>IF(AND(Y$2&gt;=$C28,Y$2&lt;=$C28+$D28-1),TRUE,FALSE)</formula>
+  <conditionalFormatting sqref="Y38:AD38">
+    <cfRule type="expression" dxfId="0" priority="41">
+      <formula>IF(AND(Y$2&gt;=$C38,Y$2&lt;=$C38+$D38-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="42">
+      <formula>IF(AND(Y$2&gt;=$C38,Y$2&lt;=$C38+$D38-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="43">
+      <formula>IF(AND(Y$2&gt;=$C38,Y$2&lt;=$C38+$D38-1),TRUE,FALSE)</formula>
     </cfRule>
     <cfRule type="expression" priority="44">
-      <formula>IF(AND(Y$2&gt;=$C28,Y$2&lt;=$C28+$D28-1),TRUE,FALSE)</formula>
+      <formula>IF(AND(Y$2&gt;=$C38,Y$2&lt;=$C38+$D38-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y29:AD29">
-    <cfRule type="expression" dxfId="1" priority="37">
-      <formula>IF(AND(Y$2&gt;=$C29,Y$2&lt;=$C29+$D29-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="38">
-      <formula>IF(AND(Y$2&gt;=$C29,Y$2&lt;=$C29+$D29-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="39">
-      <formula>IF(AND(Y$2&gt;=$C29,Y$2&lt;=$C29+$D29-1),TRUE,FALSE)</formula>
+  <conditionalFormatting sqref="Y39:AD39">
+    <cfRule type="expression" dxfId="0" priority="37">
+      <formula>IF(AND(Y$2&gt;=$C39,Y$2&lt;=$C39+$D39-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="38">
+      <formula>IF(AND(Y$2&gt;=$C39,Y$2&lt;=$C39+$D39-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="39">
+      <formula>IF(AND(Y$2&gt;=$C39,Y$2&lt;=$C39+$D39-1),TRUE,FALSE)</formula>
     </cfRule>
     <cfRule type="expression" priority="40">
-      <formula>IF(AND(Y$2&gt;=$C29,Y$2&lt;=$C29+$D29-1),TRUE,FALSE)</formula>
+      <formula>IF(AND(Y$2&gt;=$C39,Y$2&lt;=$C39+$D39-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y30:AD30">
-    <cfRule type="expression" dxfId="1" priority="33">
-      <formula>IF(AND(Y$2&gt;=$C30,Y$2&lt;=$C30+$D30-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="34">
-      <formula>IF(AND(Y$2&gt;=$C30,Y$2&lt;=$C30+$D30-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="35">
-      <formula>IF(AND(Y$2&gt;=$C30,Y$2&lt;=$C30+$D30-1),TRUE,FALSE)</formula>
+  <conditionalFormatting sqref="Y40:AD40">
+    <cfRule type="expression" dxfId="0" priority="33">
+      <formula>IF(AND(Y$2&gt;=$C40,Y$2&lt;=$C40+$D40-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="34">
+      <formula>IF(AND(Y$2&gt;=$C40,Y$2&lt;=$C40+$D40-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="35">
+      <formula>IF(AND(Y$2&gt;=$C40,Y$2&lt;=$C40+$D40-1),TRUE,FALSE)</formula>
     </cfRule>
     <cfRule type="expression" priority="36">
-      <formula>IF(AND(Y$2&gt;=$C30,Y$2&lt;=$C30+$D30-1),TRUE,FALSE)</formula>
+      <formula>IF(AND(Y$2&gt;=$C40,Y$2&lt;=$C40+$D40-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y31:AD31">
-    <cfRule type="expression" dxfId="1" priority="29">
-      <formula>IF(AND(Y$2&gt;=$C31,Y$2&lt;=$C31+$D31-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="30">
-      <formula>IF(AND(Y$2&gt;=$C31,Y$2&lt;=$C31+$D31-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="31">
-      <formula>IF(AND(Y$2&gt;=$C31,Y$2&lt;=$C31+$D31-1),TRUE,FALSE)</formula>
+  <conditionalFormatting sqref="Y41:AD41">
+    <cfRule type="expression" dxfId="0" priority="29">
+      <formula>IF(AND(Y$2&gt;=$C41,Y$2&lt;=$C41+$D41-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="30">
+      <formula>IF(AND(Y$2&gt;=$C41,Y$2&lt;=$C41+$D41-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="31">
+      <formula>IF(AND(Y$2&gt;=$C41,Y$2&lt;=$C41+$D41-1),TRUE,FALSE)</formula>
     </cfRule>
     <cfRule type="expression" priority="32">
-      <formula>IF(AND(Y$2&gt;=$C31,Y$2&lt;=$C31+$D31-1),TRUE,FALSE)</formula>
+      <formula>IF(AND(Y$2&gt;=$C41,Y$2&lt;=$C41+$D41-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH33:AN33">
-    <cfRule type="expression" dxfId="1" priority="25">
-      <formula>IF(AND(AH$2&gt;=$C33,AH$2&lt;=$C33+$D33-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="26">
-      <formula>IF(AND(AH$2&gt;=$C33,AH$2&lt;=$C33+$D33-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="27">
-      <formula>IF(AND(AH$2&gt;=$C33,AH$2&lt;=$C33+$D33-1),TRUE,FALSE)</formula>
+  <conditionalFormatting sqref="AH43:AN43">
+    <cfRule type="expression" dxfId="0" priority="25">
+      <formula>IF(AND(AH$2&gt;=$C43,AH$2&lt;=$C43+$D43-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="26">
+      <formula>IF(AND(AH$2&gt;=$C43,AH$2&lt;=$C43+$D43-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="27">
+      <formula>IF(AND(AH$2&gt;=$C43,AH$2&lt;=$C43+$D43-1),TRUE,FALSE)</formula>
     </cfRule>
     <cfRule type="expression" priority="28">
-      <formula>IF(AND(AH$2&gt;=$C33,AH$2&lt;=$C33+$D33-1),TRUE,FALSE)</formula>
+      <formula>IF(AND(AH$2&gt;=$C43,AH$2&lt;=$C43+$D43-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH34:AN34">
-    <cfRule type="expression" dxfId="1" priority="21">
-      <formula>IF(AND(AH$2&gt;=$C34,AH$2&lt;=$C34+$D34-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="22">
-      <formula>IF(AND(AH$2&gt;=$C34,AH$2&lt;=$C34+$D34-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="23">
-      <formula>IF(AND(AH$2&gt;=$C34,AH$2&lt;=$C34+$D34-1),TRUE,FALSE)</formula>
+  <conditionalFormatting sqref="AH44:AN44">
+    <cfRule type="expression" dxfId="0" priority="21">
+      <formula>IF(AND(AH$2&gt;=$C44,AH$2&lt;=$C44+$D44-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="22">
+      <formula>IF(AND(AH$2&gt;=$C44,AH$2&lt;=$C44+$D44-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="23">
+      <formula>IF(AND(AH$2&gt;=$C44,AH$2&lt;=$C44+$D44-1),TRUE,FALSE)</formula>
     </cfRule>
     <cfRule type="expression" priority="24">
-      <formula>IF(AND(AH$2&gt;=$C34,AH$2&lt;=$C34+$D34-1),TRUE,FALSE)</formula>
+      <formula>IF(AND(AH$2&gt;=$C44,AH$2&lt;=$C44+$D44-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH35:AN35">
-    <cfRule type="expression" dxfId="1" priority="17">
-      <formula>IF(AND(AH$2&gt;=$C35,AH$2&lt;=$C35+$D35-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="18">
-      <formula>IF(AND(AH$2&gt;=$C35,AH$2&lt;=$C35+$D35-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="19">
-      <formula>IF(AND(AH$2&gt;=$C35,AH$2&lt;=$C35+$D35-1),TRUE,FALSE)</formula>
+  <conditionalFormatting sqref="AH45:AN45">
+    <cfRule type="expression" dxfId="0" priority="17">
+      <formula>IF(AND(AH$2&gt;=$C45,AH$2&lt;=$C45+$D45-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="18">
+      <formula>IF(AND(AH$2&gt;=$C45,AH$2&lt;=$C45+$D45-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="19">
+      <formula>IF(AND(AH$2&gt;=$C45,AH$2&lt;=$C45+$D45-1),TRUE,FALSE)</formula>
     </cfRule>
     <cfRule type="expression" priority="20">
-      <formula>IF(AND(AH$2&gt;=$C35,AH$2&lt;=$C35+$D35-1),TRUE,FALSE)</formula>
+      <formula>IF(AND(AH$2&gt;=$C45,AH$2&lt;=$C45+$D45-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH36:AN36">
-    <cfRule type="expression" dxfId="1" priority="13">
-      <formula>IF(AND(AH$2&gt;=$C36,AH$2&lt;=$C36+$D36-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="14">
-      <formula>IF(AND(AH$2&gt;=$C36,AH$2&lt;=$C36+$D36-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="15">
-      <formula>IF(AND(AH$2&gt;=$C36,AH$2&lt;=$C36+$D36-1),TRUE,FALSE)</formula>
+  <conditionalFormatting sqref="AH46:AN46">
+    <cfRule type="expression" dxfId="0" priority="13">
+      <formula>IF(AND(AH$2&gt;=$C46,AH$2&lt;=$C46+$D46-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="14">
+      <formula>IF(AND(AH$2&gt;=$C46,AH$2&lt;=$C46+$D46-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="15">
+      <formula>IF(AND(AH$2&gt;=$C46,AH$2&lt;=$C46+$D46-1),TRUE,FALSE)</formula>
     </cfRule>
     <cfRule type="expression" priority="16">
-      <formula>IF(AND(AH$2&gt;=$C36,AH$2&lt;=$C36+$D36-1),TRUE,FALSE)</formula>
+      <formula>IF(AND(AH$2&gt;=$C46,AH$2&lt;=$C46+$D46-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH37:AN37">
-    <cfRule type="expression" dxfId="1" priority="9">
-      <formula>IF(AND(AH$2&gt;=$C37,AH$2&lt;=$C37+$D37-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="10">
-      <formula>IF(AND(AH$2&gt;=$C37,AH$2&lt;=$C37+$D37-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="11">
-      <formula>IF(AND(AH$2&gt;=$C37,AH$2&lt;=$C37+$D37-1),TRUE,FALSE)</formula>
+  <conditionalFormatting sqref="AH47:AN47">
+    <cfRule type="expression" dxfId="0" priority="9">
+      <formula>IF(AND(AH$2&gt;=$C47,AH$2&lt;=$C47+$D47-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="10">
+      <formula>IF(AND(AH$2&gt;=$C47,AH$2&lt;=$C47+$D47-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="11">
+      <formula>IF(AND(AH$2&gt;=$C47,AH$2&lt;=$C47+$D47-1),TRUE,FALSE)</formula>
     </cfRule>
     <cfRule type="expression" priority="12">
-      <formula>IF(AND(AH$2&gt;=$C37,AH$2&lt;=$C37+$D37-1),TRUE,FALSE)</formula>
+      <formula>IF(AND(AH$2&gt;=$C47,AH$2&lt;=$C47+$D47-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH40:AN40">
-    <cfRule type="expression" dxfId="1" priority="4">
-      <formula>IF(AND(AH$2&gt;=$C40,AH$2&lt;=$C40+$D40-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>IF(AND(AH$2&gt;=$C40,AH$2&lt;=$C40+$D40-1),TRUE,FALSE)</formula>
+  <conditionalFormatting sqref="AH50:AN50">
+    <cfRule type="expression" dxfId="0" priority="3">
+      <formula>IF(AND(AH$2&gt;=$C50,AH$2&lt;=$C50+$D50-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="4">
+      <formula>IF(AND(AH$2&gt;=$C50,AH$2&lt;=$C50+$D50-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL44:AR44">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>IF(AND(AL$2&gt;=$C44,AL$2&lt;=$C44+$D44-1),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>IF(AND(AL$2&gt;=$C44,AL$2&lt;=$C44+$D44-1),TRUE,FALSE)</formula>
+  <conditionalFormatting sqref="AL54:AR54">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>IF(AND(AL$2&gt;=$C54,AL$2&lt;=$C54+$D54-1),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>IF(AND(AL$2&gt;=$C54,AL$2&lt;=$C54+$D54-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:AU15">
-    <cfRule type="expression" dxfId="0" priority="62">
+    <cfRule type="expression" dxfId="1" priority="62">
       <formula>IF(AND(E$2&gt;=$C3,E$2&lt;=$C3+$D3-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:AU22 E32:AU32 E24:AU24 E41:AU41">
-    <cfRule type="expression" dxfId="0" priority="59">
+  <conditionalFormatting sqref="E3:AU22 E51:AU51 E42:AU42 E34:AU34">
+    <cfRule type="expression" dxfId="1" priority="59">
       <formula>IF(AND(E$2&gt;=$C3,E$2&lt;=$C3+$D3-1),TRUE,FALSE)</formula>
     </cfRule>
     <cfRule type="expression" priority="60">
       <formula>IF(AND(E$2&gt;=$C3,E$2&lt;=$C3+$D3-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:AU22 E45:AU51 E53:AU54 E32:AU32 E56:AU113 E38:AU39 E41:AU43 E24:AU24">
-    <cfRule type="expression" dxfId="1" priority="58">
+  <conditionalFormatting sqref="E3:AU22 E34:AU34 E51:AU53 E48:AU49 E63:AU113 E55:AU61 E42:AU42">
+    <cfRule type="expression" dxfId="0" priority="58">
       <formula>IF(AND(E$2&gt;=$C3,E$2&lt;=$C3+$D3-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:AY22 E45:AY51 E53:AY54 E32:AY32 E56:AY94 E38:AY39 E41:AY43 E24:AY24">
-    <cfRule type="expression" dxfId="1" priority="57">
+  <conditionalFormatting sqref="E3:AY22 E34:AY34 E51:AY53 E48:AY49 E63:AY94 E55:AY61 E42:AY42">
+    <cfRule type="expression" dxfId="0" priority="57">
       <formula>IF(AND(E$2&gt;=$C3,E$2&lt;=$C3+$D3-1),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>